<commit_message>
design tasks trial commit
</commit_message>
<xml_diff>
--- a/Lyngr.COM/Requirements/Design_Tasks.xlsx
+++ b/Lyngr.COM/Requirements/Design_Tasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DESIGN- Screens" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="405">
   <si>
     <t>Screen Name</t>
   </si>
@@ -1228,6 +1228,15 @@
   </si>
   <si>
     <t xml:space="preserve">Backround of a  Map with previous filters applied and applicable spots. Top Menu- with search icon, menu icon, logo/title, Bottom Menu ? Navigation is done by touch.  filter pullout, </t>
+  </si>
+  <si>
+    <t>ALL SCREENS</t>
+  </si>
+  <si>
+    <t>incomplete</t>
+  </si>
+  <si>
+    <t>HIGH</t>
   </si>
 </sst>
 </file>
@@ -1587,7 +1596,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1597,7 +1606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3302,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3532,7 +3541,18 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D12" t="s">
+        <v>403</v>
+      </c>
+      <c r="E12" t="s">
+        <v>285</v>
+      </c>
+      <c r="F12" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13">

</xml_diff>